<commit_message>
cds Primary diagnosis fixed
</commit_message>
<xml_diff>
--- a/InputFiles/TC02_CDS_Filter_Prim_Diag_AcinarCellCarcinoma.xlsx
+++ b/InputFiles/TC02_CDS_Filter_Prim_Diag_AcinarCellCarcinoma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\Sofia0629\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\sofia0717new\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB64F11-789A-4B86-8B84-E62C0EC4DC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A121EC6-FBBD-4AF3-AD76-CCC1FC13E636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -63,22 +63,6 @@
     <t>TC02_CDS_Filter_Prim_Diag_AcinarCellCarcinoma_WebData.xlsx</t>
   </si>
   <si>
-    <t>MATCH (f:file)
-MATCH (g:genomic_info)
- MATCH (diag:diagnosis)--&gt;(p)
-WHERE diag.primary_diagnosis in ['Acinar cell carcinoma']
-MATCH (g)--&gt;(f:file)--&gt;(samp:sample)--&gt;(p:participant)--&gt;(s:study)
-WITH p, s, collect(distinct samp.sample_id) as samp
-RETURN 
-    coalesce(p.participant_id,'') as `Participant ID`,
-    coalesce(s.study_name, '') as `Study Name`,
-    coalesce(s.phs_accession,'') as `Accession`,
-    coalesce(p.gender,'') as `Gender`,
-    coalesce(apoc.text.join(samp, ','), '') as `Samples`
-ORDER BY `Participant ID`
-LIMIT 100</t>
-  </si>
-  <si>
     <t>MATCH (g:genomic_info)
 MATCH (diag:diagnosis)--&gt;(p)
 WHERE diag.primary_diagnosis in ['Acinar cell carcinoma']
@@ -120,6 +104,27 @@
     coalesce(f.file_type, '') as `File Type`
    ORDER By f.file_name 
    LIMIT 100</t>
+  </si>
+  <si>
+    <t>MATCH (p:participant)--&gt;(s:study)
+OPTIONAL MATCH (samp:sample)--&gt;(p)
+OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp)&lt;--(f:file)
+OPTIONAL MATCH (f)&lt;--(g:genomic_info)
+WITH s, p, samp, f, g, diag
+WHERE diag.primary_diagnosis in ['Acinar cell carcinoma']
+WITH p
+OPTIONAL MATCH (p)--&gt;(s:study)
+OPTIONAL MATCH (samp:sample)--&gt;(p)
+WITH s, p, apoc.coll.sort(collect(distinct samp.sample_id)) as samp
+RETURN 
+coalesce(p.participant_id,'') as `Participant ID`,
+coalesce(s.study_name, '') as `Study Name`,
+coalesce(s.phs_accession,'') as `Accession`,
+coalesce(p.gender,'') as `Gender`,
+coalesce(apoc.text.join(samp, ','), '') as `Samples`
+ORDER BY p.participant_id
+LIMIT 100</t>
   </si>
 </sst>
 </file>
@@ -502,7 +507,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,15 +535,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="252" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="330.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -552,10 +557,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -569,10 +574,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>

</xml_diff>